<commit_message>
Added image of campagin from 2020
</commit_message>
<xml_diff>
--- a/DnData/D20/MYLUCK_20Camp.xlsx
+++ b/DnData/D20/MYLUCK_20Camp.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e9bc99d395ef8c9/Desktop/Resources/DnD/DnD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\DnData\D20\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="220" documentId="114_{89348119-2DAE-421F-ABCA-8CE52759B921}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BB278949-B94A-4735-9395-76716F2E7358}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871949D7-CB5B-467D-BEA1-BB65A0F7D441}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{555EC10F-2DA9-4A2E-ABDF-A872F8AFBE1A}"/>
   </bookViews>
@@ -33,15 +33,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Number Rolled</t>
   </si>
   <si>
     <t xml:space="preserve">       </t>
-  </si>
-  <si>
-    <t>Aliander</t>
   </si>
   <si>
     <t>Instances Rolled</t>
@@ -1021,7 +1018,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Instances Rolled V. Value</a:t>
+              <a:t>Instances Rolled V. Value - Camp. 2020</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3622,8 +3619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8EF6D9-5AD5-43CA-9518-DC5AA8E532CB}">
   <dimension ref="A1:V25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3639,10 +3636,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
       </c>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
@@ -3953,7 +3950,7 @@
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B22">
         <f>SUM(B2:B21)</f>
@@ -3965,7 +3962,7 @@
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B24">
         <f>SUM(B2:B11)</f>
@@ -3978,7 +3975,7 @@
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B25">
         <f>SUM(B12:B21)</f>
@@ -3987,9 +3984,6 @@
       <c r="C25" s="3">
         <f>SUM(C12:C21)</f>
         <v>40.256410256410255</v>
-      </c>
-      <c r="T25" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>